<commit_message>
#10 compare mwpersistence with WikiWho
</commit_message>
<xml_diff>
--- a/wikiwho/tests/test_wikiwho_simple.xlsx
+++ b/wikiwho/tests/test_wikiwho_simple.xlsx
@@ -362,7 +362,7 @@
     <t>]</t>
   </si>
   <si>
-    <t>FOR_INITIAL_PIERCINGS.pdf Glass for initial piercing]&lt;/ref&gt;</t>
+    <t>Glass for initial piercing]&lt;/ref&gt;</t>
   </si>
   <si>
     <t>366156901</t>
@@ -2584,8 +2584,8 @@
   </sheetPr>
   <dimension ref="1:241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D195" activeCellId="0" sqref="D195"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
update test excel for mwpersistence
</commit_message>
<xml_diff>
--- a/wikiwho/tests/test_wikiwho_simple.xlsx
+++ b/wikiwho/tests/test_wikiwho_simple.xlsx
@@ -425,7 +425,7 @@
     <t>total</t>
   </si>
   <si>
-    <t>although the average total length is much less.&lt;ref name=</t>
+    <t>although the average total length is much less</t>
   </si>
   <si>
     <t>520263878</t>
@@ -1630,7 +1630,7 @@
     <t>459217814</t>
   </si>
   <si>
-    <t>Quraysh and use of bribes.&lt;ref name =</t>
+    <t>Quraysh and use of bribes</t>
   </si>
   <si>
     <t>203173838</t>
@@ -2584,8 +2584,8 @@
   </sheetPr>
   <dimension ref="1:241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E164" activeCellId="0" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
test article name is changed (South_Western_Main_Line -> South_Western_main_line)
</commit_message>
<xml_diff>
--- a/wikiwho/tests/test_wikiwho_simple.xlsx
+++ b/wikiwho/tests/test_wikiwho_simple.xlsx
@@ -1952,7 +1952,7 @@
     <t>Yegorov and Feoktistov, was launched</t>
   </si>
   <si>
-    <t>South_Western_Main_Line</t>
+    <t>South_Western_main_line</t>
   </si>
   <si>
     <t>286</t>
@@ -2584,8 +2584,8 @@
   </sheetPr>
   <dimension ref="1:241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E164" activeCellId="0" sqref="E164"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A206" activeCellId="0" sqref="A206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
klm destinations name has changed
</commit_message>
<xml_diff>
--- a/wikiwho/tests/test_wikiwho_simple.xlsx
+++ b/wikiwho/tests/test_wikiwho_simple.xlsx
@@ -5,809 +5,820 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="test_wikiwho_simple_" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="753">
   <si>
-    <t>Article</t>
-  </si>
-  <si>
-    <t>Number of revisions in this article</t>
-  </si>
-  <si>
-    <t>Revision for whose words the authorship is determined (starting revision)</t>
-  </si>
-  <si>
-    <t>Token</t>
-  </si>
-  <si>
-    <t>Context to identify token in starting revision</t>
-  </si>
-  <si>
-    <t>Correct</t>
-  </si>
-  <si>
-    <t>Amstrad CPC</t>
-  </si>
-  <si>
-    <t>863</t>
-  </si>
-  <si>
-    <t>574978117</t>
-  </si>
-  <si>
-    <t>support</t>
-  </si>
-  <si>
-    <t>enhancements include the support of analogue</t>
-  </si>
-  <si>
-    <t>351259464</t>
-  </si>
-  <si>
-    <t>rom</t>
-  </si>
-  <si>
-    <t>equipped with an on-board ROM</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>''Amstrad Spain'') during a short time in 1985. Its</t>
-  </si>
-  <si>
-    <t>445260692</t>
-  </si>
-  <si>
-    <t>968</t>
-  </si>
-  <si>
-    <t>routines and explanations (Soft 968)&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>353535318</t>
-  </si>
-  <si>
-    <t>]]</t>
-  </si>
-  <si>
-    <t>custom-designed [[gate array]] to generate</t>
-  </si>
-  <si>
-    <t>353723083</t>
-  </si>
-  <si>
-    <t>comprising</t>
-  </si>
-  <si>
-    <t>[[AMSDOS]] format, comprising 2 kB directory and</t>
-  </si>
-  <si>
-    <t>100699489</t>
-  </si>
-  <si>
-    <t>Antarctica</t>
-  </si>
-  <si>
-    <t>7207</t>
-  </si>
-  <si>
-    <t>480465006</t>
-  </si>
-  <si>
-    <t>The</t>
-  </si>
-  <si>
-    <t>biodiversity in Antarctica. The Antarctic Treaty Consultative</t>
-  </si>
-  <si>
-    <t>439048860</t>
-  </si>
-  <si>
-    <t>7888558</t>
-  </si>
-  <si>
-    <t>|newspaper=BBC News|publisher=British Broadcasting Corporation|url=http://news.bbc.co.uk/2/hi/science/nature/7888558.stm|accessdate=22 October 2011}}&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>271065008</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>of flowering plants, both found in the Antarctic</t>
-  </si>
-  <si>
-    <t>39545040</t>
-  </si>
-  <si>
-    <t>after</t>
-  </si>
-  <si>
-    <t>The [[Weddell Seal]], a "[[true seal]]", is named after [[James Weddell|Sir James Weddell]]</t>
-  </si>
-  <si>
-    <t>48349017</t>
-  </si>
-  <si>
-    <t>issued</t>
-  </si>
-  <si>
-    <t>"wintered over" bar issued to those who remain</t>
-  </si>
-  <si>
-    <t>20732894</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>in area after [[Asia]], [[Africa]], [[North America]]</t>
-  </si>
-  <si>
-    <t>108729158</t>
-  </si>
-  <si>
-    <t>Apollo 11</t>
-  </si>
-  <si>
-    <t>5332</t>
-  </si>
-  <si>
-    <t>480561960</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>Shadow of the Moon: A Challenging Journey to Tranquillity]]</t>
-  </si>
-  <si>
-    <t>302273677</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>[[Mission patch|patch]] of ''Apollo 11'' was designed by Collins, who wanted a symbol</t>
-  </si>
-  <si>
-    <t>49493998</t>
-  </si>
-  <si>
-    <t>Mankind</t>
-  </si>
-  <si>
-    <t>Archive short film|id=gov.archives.arc.7500|name="Apollo 11: One Giant Leap for Mankind"}}</t>
-  </si>
-  <si>
-    <t>477670909</t>
-  </si>
-  <si>
-    <t>judge</t>
-  </si>
-  <si>
-    <t>engineers would be able to judge its post-landing condition.</t>
-  </si>
-  <si>
-    <t>5329985</t>
-  </si>
-  <si>
-    <t>was</t>
-  </si>
-  <si>
-    <t>Herald}}&lt;/ref&gt; The signal was received at [[Goldstone Deep Space</t>
-  </si>
-  <si>
-    <t>68837751</t>
-  </si>
-  <si>
-    <t>presentation</t>
-  </si>
-  <si>
-    <t>President [[Spiro T. Agnew]] honored each astronaut with a presentation of the [[Presidential Medal</t>
-  </si>
-  <si>
-    <t>57847666</t>
-  </si>
-  <si>
-    <t>Armenian Genocide</t>
-  </si>
-  <si>
-    <t>7359</t>
-  </si>
-  <si>
-    <t>479933583</t>
-  </si>
-  <si>
-    <t>historical and communal heritage was yet another key purpose</t>
-  </si>
-  <si>
-    <t>258281101</t>
-  </si>
-  <si>
-    <t>Detlev</t>
-  </si>
-  <si>
-    <t>their actions.&lt;ref&gt;Türkei By Klaus-Detlev. Grothusen.&lt;/ref&gt; However,</t>
-  </si>
-  <si>
-    <t>125989406</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
-    <t>waves of [[ethnic cleansing]], by both sides. Some foreign policy</t>
-  </si>
-  <si>
-    <t>202978608</t>
-  </si>
-  <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>flattened, and, in several cities (e.g. Van), Armenian quarters were demolished</t>
-  </si>
-  <si>
-    <t>Aleppo</t>
-  </si>
-  <si>
-    <t>File:017.jpg|Aleppo, Syria.</t>
-  </si>
-  <si>
-    <t>346639084</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>of World War I | volume = iv |pages = 1153–57}}&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>170337078</t>
-  </si>
-  <si>
-    <t>Barack_Obama</t>
-  </si>
-  <si>
-    <t>21827</t>
-  </si>
-  <si>
-    <t>480773610</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>==Notes==</t>
-  </si>
-  <si>
-    <t>75771107</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>|birth_name    = Barack Hussein Obama II</t>
-  </si>
-  <si>
-    <t>431666999</t>
-  </si>
-  <si>
-    <t>earning</t>
-  </si>
-  <si>
-    <t>Chicago before earning his [[Juris Doctor|law degree]].</t>
-  </si>
-  <si>
-    <t>266793108</t>
-  </si>
-  <si>
-    <t>Muammar</t>
-  </si>
-  <si>
-    <t>In March 2011, as forces loyal to [[Muammar Gaddafi]] advanced on rebels across</t>
-  </si>
-  <si>
-    <t>420730024</t>
-  </si>
-  <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>News|accessdate=May 4, 2011}}&lt;/ref&gt; and from many countries around the world.</t>
-  </si>
-  <si>
-    <t>427329153</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>which Obama wanted Congress to approve by the end of 2009.&lt;ref name</t>
-  </si>
-  <si>
-    <t>312905509</t>
-  </si>
-  <si>
-    <t>Bioglass</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>480327915</t>
-  </si>
-  <si>
-    <t>crucial</t>
-  </si>
-  <si>
-    <t>(glass)|Annealing]] is a crucial step in forming</t>
-  </si>
-  <si>
-    <t>363578879</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>Glass for initial piercing]&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>366156901</t>
-  </si>
-  <si>
-    <t>seamlessly</t>
-  </si>
-  <si>
-    <t>completely synthetic materials that seamlessly bonds to bone.</t>
-  </si>
-  <si>
-    <t>469639985</t>
-  </si>
-  <si>
-    <t>others</t>
-  </si>
-  <si>
-    <t>nonadhering [[fibrous tissue]], and others are completely resorbed</t>
-  </si>
-  <si>
-    <t>0854045724</t>
-  </si>
-  <si>
-    <t>Royal Society of Chemistry, 2002 ISBN 0854045724&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>studied</t>
-  </si>
-  <si>
-    <t>the ﬁrst composition studied! Later studies by Hench</t>
-  </si>
-  <si>
-    <t>Bothrops_jararaca</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>559837585</t>
-  </si>
-  <si>
-    <t>enzyme</t>
-  </si>
-  <si>
-    <t>haemocoagulase enzyme derived from the venom</t>
-  </si>
-  <si>
-    <t>518970879</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>sea level to over 1,000 m altitude</t>
-  </si>
-  <si>
-    <t>102213719</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>although the average total length is much less</t>
-  </si>
-  <si>
-    <t>520263878</t>
-  </si>
-  <si>
-    <t>thumb</t>
-  </si>
-  <si>
-    <t>[[File:Jararaca.jpg|thumb|''Bothrops</t>
-  </si>
-  <si>
-    <t>483034603</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>]]. The [[Specific name (zoology)|</t>
-  </si>
-  <si>
-    <t>520255214</t>
-  </si>
-  <si>
-    <t>deciduous</t>
-  </si>
-  <si>
-    <t>The species prefers deciduous tropical forests and savanna country, as well as</t>
-  </si>
-  <si>
-    <t>Chlorine</t>
-  </si>
-  <si>
-    <t>3476</t>
-  </si>
-  <si>
-    <t>574162673</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>under standard conditions, where it</t>
-  </si>
-  <si>
-    <t>74942734</t>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>2|-}} + 2 OH&lt;sup&gt;</t>
-  </si>
-  <si>
-    <t>302318119</t>
-  </si>
-  <si>
-    <t>hcl</t>
-  </si>
-  <si>
-    <t>:4 HCl + MnO&lt;sub&gt;2</t>
-  </si>
-  <si>
-    <t>190903284</t>
-  </si>
-  <si>
-    <t>web</t>
-  </si>
-  <si>
-    <t>http://web.lemoyne.edu/~giunta/thenard.html|quote</t>
-  </si>
-  <si>
-    <t>224392842</t>
-  </si>
-  <si>
-    <t>dating</t>
-  </si>
-  <si>
-    <t>including dating ice and</t>
-  </si>
-  <si>
-    <t>185169</t>
-  </si>
-  <si>
-    <t>Circumcision</t>
-  </si>
-  <si>
-    <t>9983</t>
-  </si>
-  <si>
-    <t>480178699</t>
-  </si>
-  <si>
-    <t>As</t>
-  </si>
-  <si>
-    <t>As a demonstration of one's ability to endure pain</t>
-  </si>
-  <si>
-    <t>411424427</t>
-  </si>
-  <si>
-    <t>surrounds</t>
-  </si>
-  <si>
-    <t>Considerable controversy surrounds neonatal circumcision.</t>
-  </si>
-  <si>
-    <t>95557351</t>
-  </si>
-  <si>
-    <t>Level.png|thumb|300px|Prevalence of circumcision by country]]</t>
-  </si>
-  <si>
-    <t>442576809</t>
-  </si>
-  <si>
-    <t>While</t>
-  </si>
-  <si>
-    <t>While the same study found</t>
-  </si>
-  <si>
-    <t>475661433</t>
-  </si>
-  <si>
-    <t>cases</t>
-  </si>
-  <si>
-    <t>pathological phimosis, and in most cases is not serious;</t>
-  </si>
-  <si>
-    <t>245248120</t>
-  </si>
-  <si>
-    <t>The circumcision rate has declined sharply in Australia</t>
-  </si>
-  <si>
-    <t>208807165</t>
-  </si>
-  <si>
-    <t>Communist Party of China</t>
-  </si>
-  <si>
-    <t>2845</t>
-  </si>
-  <si>
-    <t>574338590</t>
-  </si>
-  <si>
-    <t>elects</t>
-  </si>
-  <si>
-    <t>Central Committee in turn elects the [[Politburo</t>
-  </si>
-  <si>
-    <t>417950</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>[[File:Location of the First Congress</t>
-  </si>
-  <si>
-    <t>372845974</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>perspectives {{which|date=December 2012}}, brings</t>
-  </si>
-  <si>
-    <t>528932365</t>
-  </si>
-  <si>
-    <t>translated</t>
-  </si>
-  <si>
-    <t>Communist Party'' translated by Joshua A. Fogel</t>
-  </si>
-  <si>
-    <t>535588545</t>
-  </si>
-  <si>
-    <t>Democritus</t>
-  </si>
-  <si>
-    <t>4076</t>
-  </si>
-  <si>
-    <t>574425926</t>
-  </si>
-  <si>
-    <t>sextus</t>
-  </si>
-  <si>
-    <t>|Sextus]] vii.138.&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>302274852</t>
-  </si>
-  <si>
-    <t>with the insight that space by itself</t>
-  </si>
-  <si>
-    <t>265011480</t>
-  </si>
-  <si>
-    <t>king</t>
-  </si>
-  <si>
-    <t>than become a king of Persia'.”</t>
-  </si>
-  <si>
-    <t>85651930</t>
-  </si>
-  <si>
-    <t>3d</t>
-  </si>
-  <si>
-    <t>[[Image:Cone 3d.png|thumb|250px|right|A</t>
-  </si>
-  <si>
-    <t>212323515</t>
-  </si>
-  <si>
-    <t>explained</t>
-  </si>
-  <si>
-    <t>connections were explained by material</t>
-  </si>
-  <si>
-    <t>349346698</t>
-  </si>
-  <si>
-    <t>[[</t>
-  </si>
-  <si>
-    <t>(40): "[[Aristoxenus]] in his</t>
-  </si>
-  <si>
-    <t>563978874</t>
-  </si>
-  <si>
-    <t>Diana,_Princess_of_Wales</t>
-  </si>
-  <si>
-    <t>10690</t>
-  </si>
-  <si>
-    <t>480720027</t>
-  </si>
-  <si>
-    <t>lure</t>
-  </si>
-  <si>
-    <t>and need for play often lure them directly into harm's</t>
-  </si>
-  <si>
-    <t>8182672</t>
-  </si>
-  <si>
-    <t>constituents</t>
-  </si>
-  <si>
-    <t>bringing home to many of our constituents the human costs of landmines</t>
-  </si>
-  <si>
-    <t>4997218</t>
-  </si>
-  <si>
-    <t>Sandringham</t>
-  </si>
-  <si>
-    <t>fell down a staircase at Sandringham in January</t>
-  </si>
-  <si>
-    <t>467136301</t>
-  </si>
-  <si>
-    <t>or</t>
-  </si>
-  <si>
-    <t>rarely deferred to the Prince or to the Royal Family,</t>
-  </si>
-  <si>
-    <t>296041451</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
-    <t>received a lump sum settlement</t>
-  </si>
-  <si>
-    <t>103327713</t>
-  </si>
-  <si>
-    <t>Encryption</t>
-  </si>
-  <si>
-    <t>1143</t>
-  </si>
-  <si>
-    <t>573020570</t>
-  </si>
-  <si>
-    <t>}}</t>
-  </si>
-  <si>
-    <t>{{Reflist}}</t>
-  </si>
-  <si>
-    <t>268549044</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>storage.&lt;ref&gt;Robert Richardson, 2008 CSI</t>
-  </si>
-  <si>
-    <t>281904759</t>
-  </si>
-  <si>
-    <t>design</t>
-  </si>
-  <si>
-    <t>slip-up in system design or execution can</t>
-  </si>
-  <si>
-    <t>128896395</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
-  <si>
-    <t>Public-key encryption is a relatively recent</t>
-  </si>
-  <si>
-    <t>519501982</t>
-  </si>
-  <si>
-    <t>wireless</t>
-  </si>
-  <si>
-    <t>telephone]]s, [[wireless microphone]]s,</t>
-  </si>
-  <si>
-    <t>159203212</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>a [[message authentication code]] (MAC)</t>
-  </si>
-  <si>
-    <t>9238917</t>
-  </si>
-  <si>
-    <t>Eritrean Defence Forces</t>
-  </si>
-  <si>
-    <t>238</t>
-  </si>
-  <si>
-    <t>574004211</t>
-  </si>
-  <si>
-    <t>In the 16th century the port of [[Massawa]]</t>
-  </si>
-  <si>
-    <t>49373254</t>
-  </si>
-  <si>
-    <t>ምክልካል</t>
+    <t xml:space="preserve">Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of revisions in this article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision for whose words the authorship is determined (starting revision)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context to identify token in starting revision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amstrad CPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574978117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enhancements include the support of analogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">351259464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipped with an on-board ROM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">''Amstrad Spain'') during a short time in 1985. Its</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445260692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">routines and explanations (Soft 968)&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">353535318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custom-designed [[gate array]] to generate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">353723083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comprising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[AMSDOS]] format, comprising 2 kB directory and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100699489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480465006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biodiversity in Antarctica. The Antarctic Treaty Consultative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439048860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7888558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|newspaper=BBC News|publisher=British Broadcasting Corporation|url=http://news.bbc.co.uk/2/hi/science/nature/7888558.stm|accessdate=22 October 2011}}&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">271065008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of flowering plants, both found in the Antarctic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39545040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The [[Weddell Seal]], a "[[true seal]]", is named after [[James Weddell|Sir James Weddell]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48349017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"wintered over" bar issued to those who remain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20732894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in area after [[Asia]], [[Africa]], [[North America]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108729158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apollo 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480561960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow of the Moon: A Challenging Journey to Tranquillity]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302273677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Mission patch|patch]] of ''Apollo 11'' was designed by Collins, who wanted a symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49493998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mankind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archive short film|id=gov.archives.arc.7500|name="Apollo 11: One Giant Leap for Mankind"}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">477670909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">judge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineers would be able to judge its post-landing condition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5329985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herald}}&lt;/ref&gt; The signal was received at [[Goldstone Deep Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68837751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">President [[Spiro T. Agnew]] honored each astronaut with a presentation of the [[Presidential Medal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57847666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armenian Genocide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">479933583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">historical and communal heritage was yet another key purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">258281101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detlev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">their actions.&lt;ref&gt;Türkei By Klaus-Detlev. Grothusen.&lt;/ref&gt; However,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125989406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waves of [[ethnic cleansing]], by both sides. Some foreign policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202978608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flattened, and, in several cities (e.g. Van), Armenian quarters were demolished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleppo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File:017.jpg|Aleppo, Syria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">346639084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of World War I | volume = iv |pages = 1153–57}}&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170337078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barack_Obama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480773610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==Notes==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75771107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|birth_name    = Barack Hussein Obama II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">431666999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">earning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago before earning his [[Juris Doctor|law degree]].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266793108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muammar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In March 2011, as forces loyal to [[Muammar Gaddafi]] advanced on rebels across</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420730024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News|accessdate=May 4, 2011}}&lt;/ref&gt; and from many countries around the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">427329153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which Obama wanted Congress to approve by the end of 2009.&lt;ref name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">312905509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioglass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480327915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crucial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(glass)|Annealing]] is a crucial step in forming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">363578879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glass for initial piercing]&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">366156901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seamlessly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completely synthetic materials that seamlessly bonds to bone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">469639985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonadhering [[fibrous tissue]], and others are completely resorbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0854045724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royal Society of Chemistry, 2002 ISBN 0854045724&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the ﬁrst composition studied! Later studies by Hench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bothrops_jararaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">559837585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enzyme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemocoagulase enzyme derived from the venom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">518970879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sea level to over 1,000 m altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102213719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">although the average total length is much less</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520263878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[File:Jararaca.jpg|thumb|''Bothrops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">483034603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]]. The [[Specific name (zoology)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520255214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deciduous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The species prefers deciduous tropical forests and savanna country, as well as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574162673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">under standard conditions, where it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74942734</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2|-}} + 2 OH&lt;sup&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302318119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hcl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:4 HCl + MnO&lt;sub&gt;2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190903284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://web.lemoyne.edu/~giunta/thenard.html|quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224392842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">including dating ice and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circumcision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480178699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a demonstration of one's ability to endure pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">411424427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surrounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Considerable controversy surrounds neonatal circumcision.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95557351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level.png|thumb|300px|Prevalence of circumcision by country]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">442576809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While the same study found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475661433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pathological phimosis, and in most cases is not serious;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245248120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The circumcision rate has declined sharply in Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208807165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communist Party of China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574338590</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Committee in turn elects the [[Politburo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">417950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[File:Location of the First Congress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">372845974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perspectives {{which|date=December 2012}}, brings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">528932365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communist Party'' translated by Joshua A. Fogel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">535588545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democritus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574425926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sextus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Sextus]] vii.138.&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302274852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with the insight that space by itself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265011480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">king</t>
+  </si>
+  <si>
+    <t xml:space="preserve">than become a king of Persia'.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85651930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Image:Cone 3d.png|thumb|250px|right|A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">212323515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">explained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connections were explained by material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">349346698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(40): "[[Aristoxenus]] in his</t>
+  </si>
+  <si>
+    <t xml:space="preserve">563978874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diana,_Princess_of_Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480720027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and need for play often lure them directly into harm's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8182672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constituents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bringing home to many of our constituents the human costs of landmines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4997218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandringham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fell down a staircase at Sandringham in January</t>
+  </si>
+  <si>
+    <t xml:space="preserve">467136301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rarely deferred to the Prince or to the Royal Family,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296041451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">received a lump sum settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103327713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encryption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">573020570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{Reflist}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">268549044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage.&lt;ref&gt;Robert Richardson, 2008 CSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">281904759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slip-up in system design or execution can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">128896395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public-key encryption is a relatively recent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">519501982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wireless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telephone]]s, [[wireless microphone]]s,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159203212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a [[message authentication code]] (MAC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9238917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eritrean Defence Forces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574004211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 16th century the port of [[Massawa]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49373254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ምክልካል</t>
   </si>
   <si>
     <r>
-      <t>| native_name =</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| native_name =</t>
     </r>
     <r>
       <rPr>
@@ -816,7 +827,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>ምክልካል ሃይልታት ኣርትራ</t>
+      <t xml:space="preserve">ምክልካል ሃይልታት ኣርትራ</t>
     </r>
     <r>
       <rPr>
@@ -825,368 +836,368 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>&lt;br /&gt;</t>
+      <t xml:space="preserve">&lt;br /&gt;</t>
     </r>
   </si>
   <si>
-    <t>112225322</t>
-  </si>
-  <si>
-    <t>reason for the military's large size is [[conscription]]</t>
-  </si>
-  <si>
-    <t>524261200</t>
-  </si>
-  <si>
-    <t>career</t>
-  </si>
-  <si>
-    <t>composed fully of career soldiers would not</t>
-  </si>
-  <si>
-    <t>59876009</t>
-  </si>
-  <si>
-    <t>[[National Assembly of Eritrea|National Assembly]]</t>
-  </si>
-  <si>
-    <t>81318111</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>Dan| year = 1997| month</t>
-  </si>
-  <si>
-    <t>76669667</t>
-  </si>
-  <si>
-    <t>European Free Trade Association</t>
-  </si>
-  <si>
-    <t>691</t>
-  </si>
-  <si>
-    <t>573013414</t>
-  </si>
-  <si>
-    <t>direct membership in the EEA for</t>
-  </si>
-  <si>
-    <t>549063890</t>
-  </si>
-  <si>
-    <t>the Council, the European Economic</t>
-  </si>
-  <si>
-    <t>Kingdom of Norway
+    <t xml:space="preserve">112225322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reason for the military's large size is [[conscription]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">524261200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">career</t>
+  </si>
+  <si>
+    <t xml:space="preserve">composed fully of career soldiers would not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59876009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[National Assembly of Eritrea|National Assembly]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81318111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dan| year = 1997| month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76669667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Free Trade Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">573013414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direct membership in the EEA for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">549063890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the Council, the European Economic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingdom of Norway
 |</t>
   </si>
   <si>
-    <t>199684622</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>&lt;ref name=IMF_Switzerland&gt;{{cite web</t>
-  </si>
-  <si>
-    <t>569218033</t>
-  </si>
-  <si>
-    <t>european</t>
-  </si>
-  <si>
-    <t>[[File:EU and EFTA.svg|thumb|Members of the European Union (blue)</t>
-  </si>
-  <si>
-    <t>316237404</t>
-  </si>
-  <si>
-    <t>administrative</t>
-  </si>
-  <si>
-    <t>microstates have sufficient administrative capabilities to</t>
-  </si>
-  <si>
-    <t>Evolution</t>
-  </si>
-  <si>
-    <t>13706</t>
-  </si>
-  <si>
-    <t>478123979</t>
-  </si>
-  <si>
-    <t>af</t>
-  </si>
-  <si>
-    <t>[[af:Evolusie]]</t>
-  </si>
-  <si>
-    <t>22030668</t>
-  </si>
-  <si>
-    <t>1925</t>
-  </si>
-  <si>
-    <t>[[Scopes Trial]] decision of 1925 caused the subject to become very</t>
-  </si>
-  <si>
-    <t>305144970</t>
-  </si>
-  <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>as can be seen by looking at its near relatives</t>
-  </si>
-  <si>
-    <t>135770029</t>
-  </si>
-  <si>
-    <t>effect]] causes rapid speciation after an increase in [[inbreeding]]</t>
-  </si>
-  <si>
-    <t>451865800</t>
-  </si>
-  <si>
-    <t>provide</t>
-  </si>
-  <si>
-    <t>relationship as the plants provide the fungi with sugars from</t>
-  </si>
-  <si>
-    <t>135342071</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>the animal's [[germ cell]]s to produce offspring.</t>
-  </si>
-  <si>
-    <t>Geography of El Salvador</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>574195509</t>
-  </si>
-  <si>
-    <t>cia</t>
-  </si>
-  <si>
-    <t>*{{CIA World Factbook}}</t>
-  </si>
-  <si>
-    <t>269718597</t>
-  </si>
-  <si>
-    <t>econ</t>
-  </si>
-  <si>
-    <t>[[Image:El salvador econ 1980.jpg|thumb|right|300px|Economic</t>
-  </si>
-  <si>
-    <t>26684473</t>
-  </si>
-  <si>
-    <t>causes</t>
-  </si>
-  <si>
-    <t>The motion of these plates causes the area's [[earthquake]]</t>
-  </si>
-  <si>
-    <t>26684250</t>
-  </si>
-  <si>
-    <t>ocean</t>
-  </si>
-  <si>
-    <t>constituting the ocean floor are forced down, they</t>
-  </si>
-  <si>
-    <t>ranges</t>
-  </si>
-  <si>
-    <t>The mountain ranges and central plateau,</t>
-  </si>
-  <si>
-    <t>slightly</t>
-  </si>
-  <si>
-    <t>This is slightly smaller than the [[U.S. state]]</t>
-  </si>
-  <si>
-    <t>457062</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>15566</t>
-  </si>
-  <si>
-    <t>480958857</t>
-  </si>
-  <si>
-    <t>Allemagne</t>
-  </si>
-  <si>
-    <t>[[File:Pyramide Allemagne.PNG|thumb|left|Germany's [[population pyramid]] in 2005]]</t>
-  </si>
-  <si>
-    <t>396518693</t>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>===Science and technology===</t>
-  </si>
-  <si>
-    <t>43149668</t>
-  </si>
-  <si>
-    <t>central position in Europe, Germany is a transport hub</t>
-  </si>
-  <si>
-    <t>134275052</t>
-  </si>
-  <si>
-    <t>particularly</t>
-  </si>
-  <si>
-    <t>decreased in recent decades, particularly among Protestants.</t>
-  </si>
-  <si>
-    <t>466110130</t>
-  </si>
-  <si>
-    <t>air</t>
-  </si>
-  <si>
-    <t>[[Karl Benz]] helped shape modern automotive and air transportation technology</t>
-  </si>
-  <si>
-    <t>93488597</t>
-  </si>
-  <si>
-    <t>Vertreibungsverbrechen</t>
-  </si>
-  <si>
-    <t>&lt;ref&gt;Bonn : Kulturstiftung der Deutschen Vertriebenen, ''Vertreibung und Vertreibungsverbrechen</t>
-  </si>
-  <si>
-    <t>434496752</t>
-  </si>
-  <si>
-    <t>Home and Away</t>
-  </si>
-  <si>
-    <t>13035</t>
-  </si>
-  <si>
-    <t>573240275</t>
-  </si>
-  <si>
-    <t>beach</t>
-  </si>
-  <si>
-    <t>and at Fisherman's Beach, [[Collaroy]]</t>
-  </si>
-  <si>
-    <t>81543195</t>
-  </si>
-  <si>
-    <t>www</t>
-  </si>
-  <si>
-    <t>&lt;ref name="Whittingham"&gt;{{cite web|url=http://www.c21media.net/archives/117214|title=TVNZ swipes</t>
-  </si>
-  <si>
-    <t>563011743</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>''Home and Away'' from 1999-2002 and [[Trouble (TV channel)|</t>
-  </si>
-  <si>
-    <t>547651622</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>every episode. From June 2006 to November 2008</t>
-  </si>
-  <si>
-    <t>253398702</t>
-  </si>
-  <si>
-    <t>we are promoting the next episode."&lt;ref&gt;{{cite news |last</t>
-  </si>
-  <si>
-    <t>303123672</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>#Book|Home and Away: Hearts Divided]]&lt;ref&gt;</t>
-  </si>
-  <si>
-    <t>393181153</t>
-  </si>
-  <si>
-    <t>Homeopathy</t>
-  </si>
-  <si>
-    <t>9141</t>
-  </si>
-  <si>
-    <t>479765637</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>|accessdate =2007-08-04
+    <t xml:space="preserve">199684622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ref name=IMF_Switzerland&gt;{{cite web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">569218033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">european</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[File:EU and EFTA.svg|thumb|Members of the European Union (blue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">316237404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">microstates have sufficient administrative capabilities to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">478123979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">af</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[af:Evolusie]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22030668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Scopes Trial]] decision of 1925 caused the subject to become very</t>
+  </si>
+  <si>
+    <t xml:space="preserve">305144970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as can be seen by looking at its near relatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135770029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effect]] causes rapid speciation after an increase in [[inbreeding]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">451865800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relationship as the plants provide the fungi with sugars from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135342071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the animal's [[germ cell]]s to produce offspring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geography of El Salvador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">574195509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*{{CIA World Factbook}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269718597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">econ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Image:El salvador econ 1980.jpg|thumb|right|300px|Economic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26684473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">causes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The motion of these plates causes the area's [[earthquake]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26684250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ocean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constituting the ocean floor are forced down, they</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mountain ranges and central plateau,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slightly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is slightly smaller than the [[U.S. state]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">457062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480958857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allemagne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[File:Pyramide Allemagne.PNG|thumb|left|Germany's [[population pyramid]] in 2005]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">396518693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">===Science and technology===</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43149668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">central position in Europe, Germany is a transport hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134275052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">particularly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decreased in recent decades, particularly among Protestants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">466110130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Karl Benz]] helped shape modern automotive and air transportation technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93488597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertreibungsverbrechen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ref&gt;Bonn : Kulturstiftung der Deutschen Vertriebenen, ''Vertreibung und Vertreibungsverbrechen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">434496752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home and Away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">573240275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and at Fisherman's Beach, [[Collaroy]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81543195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ref name="Whittingham"&gt;{{cite web|url=http://www.c21media.net/archives/117214|title=TVNZ swipes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">563011743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">''Home and Away'' from 1999-2002 and [[Trouble (TV channel)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">547651622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">every episode. From June 2006 to November 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">253398702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we are promoting the next episode."&lt;ref&gt;{{cite news |last</t>
+  </si>
+  <si>
+    <t xml:space="preserve">303123672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Book|Home and Away: Hearts Divided]]&lt;ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">393181153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homeopathy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">479765637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|accessdate =2007-08-04
 |author =Little D
 |title =Simillimum.com</t>
   </si>
   <si>
-    <t>279280908</t>
-  </si>
-  <si>
-    <t>vitalism</t>
-  </si>
-  <si>
-    <t>Homeopathy is a [[vitalism|vitalist]] philosophy that</t>
-  </si>
-  <si>
-    <t>155021551</t>
-  </si>
-  <si>
-    <t>Ont</t>
-  </si>
-  <si>
-    <t>issue=4 |pages=126–7 |pmc=1948865 |journal=Current oncology (Toronto, Ont.) |postscript=.}}&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>468898492</t>
-  </si>
-  <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>|title=Homeopathic pharmacy: theory and practice
+    <t xml:space="preserve">279280908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vitalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homeopathy is a [[vitalism|vitalist]] philosophy that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155021551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issue=4 |pages=126–7 |pmc=1948865 |journal=Current oncology (Toronto, Ont.) |postscript=.}}&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">468898492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|title=Homeopathic pharmacy: theory and practice
  |edition=2
  |publisher=Elsevier Health Sciences
  |page=52
@@ -1194,1116 +1205,1116 @@
 }}&lt;/ref&gt; During the proving process, Hahnemann</t>
   </si>
   <si>
-    <t>280678108</t>
-  </si>
-  <si>
-    <t>conflicts</t>
-  </si>
-  <si>
-    <t>into the body and conflicts with scientific studies</t>
-  </si>
-  <si>
-    <t>155320067</t>
-  </si>
-  <si>
-    <t>where</t>
-  </si>
-  <si>
-    <t>usually diluted to the point where there are no molecules</t>
-  </si>
-  <si>
-    <t>126867887</t>
-  </si>
-  <si>
-    <t>Iraq War</t>
-  </si>
-  <si>
-    <t>14557</t>
-  </si>
-  <si>
-    <t>481109117</t>
-  </si>
-  <si>
-    <t>organization/77707.pdf&lt;/ref&gt;&lt;/small&gt;&lt;br&gt;&lt;br&gt;
+    <t xml:space="preserve">280678108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conflicts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">into the body and conflicts with scientific studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155320067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">where</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usually diluted to the point where there are no molecules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126867887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iraq War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481109117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organization/77707.pdf&lt;/ref&gt;&lt;/small&gt;&lt;br&gt;&lt;br&gt;
 '''[[Multi-National Force&amp;nbsp;– Iraq|Coalition Forces]]'''&lt;br&gt;</t>
   </si>
   <si>
-    <t>406350628</t>
-  </si>
-  <si>
-    <t>By</t>
-  </si>
-  <si>
-    <t>2010}}|242&amp;nbsp;KB}}. By Gilbert Burnham, Riyadh Lafta,</t>
-  </si>
-  <si>
-    <t>87192121</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>firefight that followed a car bomb explosion</t>
-  </si>
-  <si>
-    <t>159432579</t>
-  </si>
-  <si>
-    <t>guerrilla</t>
-  </si>
-  <si>
-    <t>sharp surge in guerrilla attacks ushered</t>
-  </si>
-  <si>
-    <t>39258112</t>
-  </si>
-  <si>
-    <t>oil fields there and the important ports, supported by warships</t>
-  </si>
-  <si>
-    <t>377143000</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>the mandate was renewed on December 18, 2007,</t>
-  </si>
-  <si>
-    <t>249204227</t>
-  </si>
-  <si>
-    <t>Islamophobia</t>
-  </si>
-  <si>
-    <t>5079</t>
-  </si>
-  <si>
-    <t>468968330</t>
-  </si>
-  <si>
-    <t>Genealogy of today's Islamophobia"]{{dead link</t>
-  </si>
-  <si>
-    <t>126647965</t>
-  </si>
-  <si>
-    <t>Islamic totalitarianism with hatred of Muslims.</t>
-  </si>
-  <si>
-    <t>462012990</t>
-  </si>
-  <si>
-    <t>&lt;ref&gt;Edward W. Said, ‘Orientalism Reconsidered’ in</t>
-  </si>
-  <si>
-    <t>205333624</t>
-  </si>
-  <si>
-    <t>each</t>
-  </si>
-  <si>
-    <t>5 December 2005.&lt;/ref&gt; He writes that each country has its extremes, citing</t>
-  </si>
-  <si>
-    <t>72557725</t>
-  </si>
-  <si>
-    <t>and [[Council of Europe]], adopted a declaration to combat "genocide,</t>
-  </si>
-  <si>
-    <t>461495849</t>
-  </si>
-  <si>
-    <t>argues</t>
-  </si>
-  <si>
-    <t>birth, is despicable", but argues that "it is not a form of</t>
-  </si>
-  <si>
-    <t>468420752</t>
-  </si>
-  <si>
-    <t>Jack the Ripper</t>
-  </si>
-  <si>
-    <t>7964</t>
-  </si>
-  <si>
-    <t>481005511</t>
-  </si>
-  <si>
-    <t>Star (London)|The Star]]'', {{Nowrap</t>
-  </si>
-  <si>
-    <t>330835839</t>
-  </si>
-  <si>
-    <t>suffered</t>
-  </si>
-  <si>
-    <t>she had suffered 39 stab wounds. The savagery</t>
-  </si>
-  <si>
-    <t>333693762</t>
-  </si>
-  <si>
-    <t>Over 300 are preserved at the Corporation of London Records</t>
-  </si>
-  <si>
-    <t>320403075</t>
-  </si>
-  <si>
-    <t>ladys</t>
-  </si>
-  <si>
-    <t>To "clip the ladys ([[sic]]) ears off" gained</t>
-  </si>
-  <si>
-    <t>7104305</t>
-  </si>
-  <si>
-    <t>Donald</t>
-  </si>
-  <si>
-    <t>Of letters regarding the case.&lt;ref&gt;[[Donald McCormick]] estimated "probably at least 2000"</t>
-  </si>
-  <si>
-    <t>cartoon by [[John Tenniel]] ({{Nowrap|22 September}}</t>
-  </si>
-  <si>
-    <t>369117194</t>
-  </si>
-  <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>24210</t>
-  </si>
-  <si>
-    <t>481376127</t>
-  </si>
-  <si>
-    <t>ref&gt;''Cambridge companion to Jesus'' by Markus N. A. Bockmuehl 2001 Cambridge Univ Press ISBN 9780521796781 pages 123-124&lt;/ref</t>
-  </si>
-  <si>
-    <t>442128421</t>
-  </si>
-  <si>
-    <t>Many of the miracles in the gospels</t>
-  </si>
-  <si>
-    <t>435999249</t>
-  </si>
-  <si>
-    <t>believe in some form of the doctrine of</t>
-  </si>
-  <si>
-    <t>452325582</t>
-  </si>
-  <si>
-    <t>0802839312</t>
-  </si>
-  <si>
-    <t>by James D. G. Dunn 2003 ISBN 0802839312 page 339&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>475463224</t>
-  </si>
-  <si>
-    <t>theories about the race of Jesus were advanced,</t>
-  </si>
-  <si>
-    <t>452097741</t>
-  </si>
-  <si>
-    <t>KLM destinations</t>
-  </si>
-  <si>
-    <t>1447</t>
-  </si>
-  <si>
-    <t>481177397</t>
-  </si>
-  <si>
-    <t>airline</t>
-  </si>
-  <si>
-    <t>[[Category:Lists of airline destinations]]</t>
-  </si>
-  <si>
-    <t>22222048</t>
-  </si>
-  <si>
-    <t>KLM</t>
-  </si>
-  <si>
-    <t>[[id:Daftar bandar udara tujuan KLM]]</t>
-  </si>
-  <si>
-    <t>82567084</t>
-  </si>
-  <si>
-    <t>scheduled</t>
-  </si>
-  <si>
-    <t>according to their scheduled services.&lt;ref name="klm"&gt;</t>
-  </si>
-  <si>
-    <t>458558522</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>bgcolor=#DCDCDC|[[Groningen Airport Eelde]] &lt;sup&gt;</t>
-  </si>
-  <si>
-    <t>458792715</t>
-  </si>
-  <si>
-    <t>FORCETOC</t>
-  </si>
-  <si>
-    <t>__FORCETOC__</t>
-  </si>
-  <si>
-    <t>459197823</t>
-  </si>
-  <si>
-    <t>[[Léopold Sédar Senghor International Airport]] &lt;sup&gt;</t>
-  </si>
-  <si>
-    <t>458732268</t>
-  </si>
-  <si>
-    <t>Lemur</t>
-  </si>
-  <si>
-    <t>2670</t>
-  </si>
-  <si>
-    <t>480536972</t>
-  </si>
-  <si>
-    <t>by</t>
-  </si>
-  <si>
-    <t>higher-level taxonomy by defining lemurs as monophyletic</t>
-  </si>
-  <si>
-    <t>357339699</t>
-  </si>
-  <si>
-    <t>will</t>
-  </si>
-  <si>
-    <t>along with their young, will share nests with other</t>
-  </si>
-  <si>
-    <t>352675913</t>
-  </si>
-  <si>
-    <t>slight</t>
-  </si>
-  <si>
-    <t>anthropoid primates due to a slight difference in the</t>
-  </si>
-  <si>
-    <t>enclosures have been observed eating [[poison</t>
-  </si>
-  <si>
-    <t>made</t>
-  </si>
-  <si>
-    <t>strides have been made in lemur studies and many</t>
-  </si>
-  <si>
-    <t>include</t>
-  </si>
-  <si>
-    <t>These traits can include seasonal fat storage,</t>
-  </si>
-  <si>
-    <t>Macedonians (ethnic group)</t>
-  </si>
-  <si>
-    <t>6117</t>
-  </si>
-  <si>
-    <t>479979735</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>pro-IMRO sympathies of the population in their cause.</t>
-  </si>
-  <si>
-    <t>464580094</t>
-  </si>
-  <si>
-    <t>The church gained autonomy from the [[Serbian Orthodox Church]]</t>
-  </si>
-  <si>
-    <t>356053363</t>
-  </si>
-  <si>
-    <t>according</t>
-  </si>
-  <si>
-    <t>of 'ancestry' which, according to Members of the Australian-Macedonian Community</t>
-  </si>
-  <si>
-    <t>75919044</t>
-  </si>
-  <si>
-    <t>organizations</t>
-  </si>
-  <si>
-    <t>the emblem of several political parties, organizations and sports clubs.</t>
-  </si>
-  <si>
-    <t>248559932</t>
-  </si>
-  <si>
-    <t>Macedonians_(ethnic_group)</t>
-  </si>
-  <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>northern Greece, and southern [[Serbia]], mostly</t>
-  </si>
-  <si>
-    <t>9088682</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>ejhg/journal</t>
-  </si>
-  <si>
-    <t>187465136</t>
-  </si>
-  <si>
-    <t>Muhammad</t>
-  </si>
-  <si>
-    <t>17413</t>
-  </si>
-  <si>
-    <t>481126024</t>
-  </si>
-  <si>
-    <t>during Muhammad's early lifetime.&lt;ref name="EoI-Muhammad"/&gt;</t>
-  </si>
-  <si>
-    <t>141764169</t>
-  </si>
-  <si>
-    <t>Unicode</t>
-  </si>
-  <si>
-    <t>|date=2009-10-01 |work=The Unicode Standard, Version 5.2</t>
-  </si>
-  <si>
-    <t>459225510</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>Abu Sufyan's troops were unprepared for the fortifications they were</t>
-  </si>
-  <si>
-    <t>152603502</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>petty or trifling. His speech was a string of cascading pearls,</t>
-  </si>
-  <si>
-    <t>459217814</t>
-  </si>
-  <si>
-    <t>Quraysh and use of bribes</t>
-  </si>
-  <si>
-    <t>203173838</t>
-  </si>
-  <si>
-    <t>pagan</t>
-  </si>
-  <si>
-    <t>The first group of pagan converts to Islam in Medina</t>
-  </si>
-  <si>
-    <t>188705740</t>
-  </si>
-  <si>
-    <t>Newberg, Oregon</t>
-  </si>
-  <si>
-    <t>287</t>
-  </si>
-  <si>
-    <t>464181136</t>
-  </si>
-  <si>
-    <t>who</t>
-  </si>
-  <si>
-    <t>'''Roger's Landing''' for Rogers who founded the settlement</t>
-  </si>
-  <si>
-    <t>341434668</t>
-  </si>
-  <si>
-    <t>[[George Fox University]], and a new campus of [[Portland Community College]]</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>|Oct low F = 43</t>
-  </si>
-  <si>
-    <t>380822459</t>
-  </si>
-  <si>
-    <t>George Fox University is the only evangelical</t>
-  </si>
-  <si>
-    <t>189288958</t>
-  </si>
-  <si>
-    <t>author=Lewis A. McArthur |year=1991</t>
-  </si>
-  <si>
-    <t>360230406</t>
-  </si>
-  <si>
-    <t>households</t>
-  </si>
-  <si>
-    <t>There were 6,099 households out of which 40.2% had children</t>
-  </si>
-  <si>
-    <t>499684</t>
-  </si>
-  <si>
-    <t>Race_and_intelligence</t>
-  </si>
-  <si>
-    <t>11041</t>
-  </si>
-  <si>
-    <t>481398958</t>
-  </si>
-  <si>
-    <t>such</t>
-  </si>
-  <si>
-    <t>[[malnutrition]], [[infectious diseases]] such as [[meningitis]],</t>
-  </si>
-  <si>
-    <t>409787246</t>
-  </si>
-  <si>
-    <t>|date=12 February 2005</t>
-  </si>
-  <si>
-    <t>478210588</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>relationship between brain size and a number of cognitive measures</t>
-  </si>
-  <si>
-    <t>353076935</t>
-  </si>
-  <si>
-    <t>org</t>
-  </si>
-  <si>
-    <t>386–98 |url=http://brain.oxfordjournals.org/</t>
-  </si>
-  <si>
-    <t>IQs do not support evolutionary theories of intelligence |first=Jelte M</t>
-  </si>
-  <si>
-    <t>systematically</t>
-  </si>
-  <si>
-    <t>culture or motivation could systematically encourage black performance on one</t>
-  </si>
-  <si>
-    <t>452766286</t>
-  </si>
-  <si>
-    <t>Rhapsody_on_a_Theme_of_Paganini</t>
-  </si>
-  <si>
-    <t>265</t>
-  </si>
-  <si>
-    <t>563616407</t>
-  </si>
-  <si>
-    <t>''Paganini'' was premiered in 1939 by [[The Royal Ballet]]</t>
-  </si>
-  <si>
-    <t>207140698</t>
-  </si>
-  <si>
-    <t>28Rachmaninoff%2C_Sergei%29|cname=Rhapsody</t>
-  </si>
-  <si>
-    <t>89480162</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>#v=onepage&amp;q&amp;f=false|accessdate=2013/03/18</t>
-  </si>
-  <si>
-    <t>545277594</t>
-  </si>
-  <si>
-    <t>guitar</t>
-  </si>
-  <si>
-    <t>been turned into a [[guitar]] player in Fokine's scenario</t>
-  </si>
-  <si>
-    <t>286273879</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>a9ly90Y3WYyiGAwekMFKnPoGJ1I&amp;hl=en&amp;ei=SJv0SfSOC5GCkQXx1aD3Cg&amp;sa=X&amp;oi=book_result&amp;ct=</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>|[[Philadelphia Orchestra]]
+    <t xml:space="preserve">406350628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010}}|242&amp;nbsp;KB}}. By Gilbert Burnham, Riyadh Lafta,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87192121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firefight that followed a car bomb explosion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159432579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guerrilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sharp surge in guerrilla attacks ushered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39258112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oil fields there and the important ports, supported by warships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">377143000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the mandate was renewed on December 18, 2007,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249204227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islamophobia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">468968330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genealogy of today's Islamophobia"]{{dead link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126647965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islamic totalitarianism with hatred of Muslims.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">462012990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ref&gt;Edward W. Said, ‘Orientalism Reconsidered’ in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">205333624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 December 2005.&lt;/ref&gt; He writes that each country has its extremes, citing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72557725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and [[Council of Europe]], adopted a declaration to combat "genocide,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">461495849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">argues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth, is despicable", but argues that "it is not a form of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">468420752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack the Ripper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481005511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star (London)|The Star]]'', {{Nowrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330835839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suffered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">she had suffered 39 stab wounds. The savagery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">333693762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over 300 are preserved at the Corporation of London Records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320403075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ladys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To "clip the ladys ([[sic]]) ears off" gained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7104305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of letters regarding the case.&lt;ref&gt;[[Donald McCormick]] estimated "probably at least 2000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartoon by [[John Tenniel]] ({{Nowrap|22 September}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">369117194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481376127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref&gt;''Cambridge companion to Jesus'' by Markus N. A. Bockmuehl 2001 Cambridge Univ Press ISBN 9780521796781 pages 123-124&lt;/ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">442128421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many of the miracles in the gospels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">435999249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">believe in some form of the doctrine of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452325582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0802839312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by James D. G. Dunn 2003 ISBN 0802839312 page 339&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475463224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theories about the race of Jesus were advanced,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452097741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of KLM destinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481177397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">airline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Category:Lists of airline destinations]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22222048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[id:Daftar bandar udara tujuan KLM]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82567084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scheduled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">according to their scheduled services.&lt;ref name="klm"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458558522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bgcolor=#DCDCDC|[[Groningen Airport Eelde]] &lt;sup&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458792715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORCETOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__FORCETOC__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">459197823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Léopold Sédar Senghor International Airport]] &lt;sup&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458732268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lemur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480536972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">higher-level taxonomy by defining lemurs as monophyletic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">357339699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">along with their young, will share nests with other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">352675913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anthropoid primates due to a slight difference in the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclosures have been observed eating [[poison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">made</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strides have been made in lemur studies and many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These traits can include seasonal fat storage,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macedonians (ethnic group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">479979735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pro-IMRO sympathies of the population in their cause.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">464580094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The church gained autonomy from the [[Serbian Orthodox Church]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">356053363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">according</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of 'ancestry' which, according to Members of the Australian-Macedonian Community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75919044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the emblem of several political parties, organizations and sports clubs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">248559932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macedonians_(ethnic_group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">northern Greece, and southern [[Serbia]], mostly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9088682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ejhg/journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">187465136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481126024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">during Muhammad's early lifetime.&lt;ref name="EoI-Muhammad"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">141764169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unicode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|date=2009-10-01 |work=The Unicode Standard, Version 5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">459225510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abu Sufyan's troops were unprepared for the fortifications they were</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152603502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">petty or trifling. His speech was a string of cascading pearls,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">459217814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quraysh and use of bribes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">203173838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pagan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first group of pagan converts to Islam in Medina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188705740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newberg, Oregon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">464181136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'''Roger's Landing''' for Rogers who founded the settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341434668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[George Fox University]], and a new campus of [[Portland Community College]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Oct low F = 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380822459</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Fox University is the only evangelical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">189288958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author=Lewis A. McArthur |year=1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">360230406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There were 6,099 households out of which 40.2% had children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">499684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race_and_intelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481398958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">such</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[malnutrition]], [[infectious diseases]] such as [[meningitis]],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">409787246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|date=12 February 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">478210588</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relationship between brain size and a number of cognitive measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">353076935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">386–98 |url=http://brain.oxfordjournals.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQs do not support evolutionary theories of intelligence |first=Jelte M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">systematically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">culture or motivation could systematically encourage black performance on one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452766286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhapsody_on_a_Theme_of_Paganini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">563616407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">''Paganini'' was premiered in 1939 by [[The Royal Ballet]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">207140698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28Rachmaninoff%2C_Sergei%29|cname=Rhapsody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89480162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#v=onepage&amp;q&amp;f=false|accessdate=2013/03/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">545277594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">been turned into a [[guitar]] player in Fokine's scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">286273879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a9ly90Y3WYyiGAwekMFKnPoGJ1I&amp;hl=en&amp;ei=SJv0SfSOC5GCkQXx1aD3Cg&amp;sa=X&amp;oi=book_result&amp;ct=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|[[Philadelphia Orchestra]]
 |align="center"|[[RCA Red Seal]]</t>
   </si>
   <si>
-    <t>448599226</t>
-  </si>
-  <si>
-    <t>Robert Hues</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>462751809</t>
-  </si>
-  <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>he was one of the</t>
-  </si>
-  <si>
-    <t>251139604</t>
-  </si>
-  <si>
-    <t>with</t>
-  </si>
-  <si>
-    <t>[[circumnavigation|circumnavigated]] the globe with Cavendish between 1586 and</t>
-  </si>
-  <si>
-    <t>printer to the Queen's Most Excellent Majestie|year=1589</t>
-  </si>
-  <si>
-    <t>solator</t>
-  </si>
-  <si>
-    <t>cui solator accessit in arca Londinensi. Quo</t>
-  </si>
-  <si>
-    <t>generally believed to be an error as no such person was known</t>
-  </si>
-  <si>
-    <t>critiqued</t>
-  </si>
-  <si>
-    <t>page=123|oclc=1981442}}, critiqued by Shirley, ''Thomas</t>
-  </si>
-  <si>
-    <t>292186344</t>
-  </si>
-  <si>
-    <t>Saturn's_moons_in_fiction</t>
-  </si>
-  <si>
-    <t>210</t>
-  </si>
-  <si>
-    <t>566618655</t>
-  </si>
-  <si>
-    <t>survivors</t>
-  </si>
-  <si>
-    <t>find possible survivors transmitting a distress signal</t>
-  </si>
-  <si>
-    <t>506114944</t>
-  </si>
-  <si>
-    <t>the Librarium Daemonicum, a repositary of the knowledge</t>
-  </si>
-  <si>
-    <t>138184340</t>
-  </si>
-  <si>
-    <t>* "Outpost of the Eons" by Dirk Wylie (pseudonym of Joseph</t>
-  </si>
-  <si>
-    <t>419171504</t>
-  </si>
-  <si>
-    <t>sourcebook ''GURPS Space: Terradyne'', the Terradyne</t>
-  </si>
-  <si>
-    <t>477980732</t>
-  </si>
-  <si>
-    <t>jpg</t>
-  </si>
-  <si>
-    <t>[[Image:Dione color south.jpg|right|80px|Dione]]</t>
-  </si>
-  <si>
-    <t>135546415</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>of human colonization and mining called "M-Base".</t>
-  </si>
-  <si>
-    <t>127975759</t>
-  </si>
-  <si>
-    <t>Sergei Korolev</t>
-  </si>
-  <si>
-    <t>893</t>
-  </si>
-  <si>
-    <t>479371650</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>Sergei Korolev.jpg|Image of 1969, 10k stamp.]][</t>
-  </si>
-  <si>
-    <t>140290515</t>
-  </si>
-  <si>
-    <t>gagarin</t>
-  </si>
-  <si>
-    <t>[http://astrotalkuk.org/2011/07/25/yuri-gagarin-statue-in-london/</t>
-  </si>
-  <si>
-    <t>444607919</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>quality checks. It was successfully launched on 3 November and the dog was placed</t>
-  </si>
-  <si>
-    <t>14531720</t>
-  </si>
-  <si>
-    <t>Vladimirov</t>
-  </si>
-  <si>
-    <t>Leonid Vladimirov related the following description of Korolev</t>
-  </si>
-  <si>
-    <t>14836512</t>
-  </si>
-  <si>
-    <t>world's first space walk. The flight very nearly ended in</t>
-  </si>
-  <si>
-    <t>Yegorov and Feoktistov, was launched</t>
-  </si>
-  <si>
-    <t>South_Western_main_line</t>
-  </si>
-  <si>
-    <t>286</t>
-  </si>
-  <si>
-    <t>480564534</t>
-  </si>
-  <si>
-    <t>[[London Waterloo station|Waterloo]] in the centre of London.</t>
-  </si>
-  <si>
-    <t>181667862</t>
-  </si>
-  <si>
-    <t>{{</t>
-  </si>
-  <si>
-    <t>==References== {{reflist}}</t>
-  </si>
-  <si>
-    <t>392467433</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>Railway]] was also formed and built a line from</t>
-  </si>
-  <si>
-    <t>184072496</t>
-  </si>
-  <si>
-    <t>Basingstoke</t>
-  </si>
-  <si>
-    <t>Reading to Portsmouth via Basingstoke and Alton but the L&amp;SWR found a</t>
-  </si>
-  <si>
-    <t>189287121</t>
-  </si>
-  <si>
-    <t>The majority of passenger services are currently operated by [[South West Trains]]</t>
-  </si>
-  <si>
-    <t>9375284</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>use its own track but, after it fell into financial difficulties,</t>
-  </si>
-  <si>
-    <t>Special Air Service</t>
-  </si>
-  <si>
-    <t>5801</t>
-  </si>
-  <si>
-    <t>572817007</t>
-  </si>
-  <si>
-    <t>free</t>
-  </si>
-  <si>
-    <t>squadrons, one [[Free French]], one [[Sacred Band</t>
-  </si>
-  <si>
-    <t>350603320</t>
-  </si>
-  <si>
-    <t>Lewes</t>
-  </si>
-  <si>
-    <t>designed by Lieutenant [[Jock Lewes]] and based on the stylised</t>
-  </si>
-  <si>
-    <t>98628757</t>
-  </si>
-  <si>
-    <t>25 March 2010|publisher=Ministry of Defence|title=Why Join the Royal</t>
-  </si>
-  <si>
-    <t>351942186</t>
-  </si>
-  <si>
-    <t>| 'B' Squadron&lt;ref&gt;Fremont-Barnes, p.4&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>Michael E|title=Encyclopaedia of Elite Forces in the Second World War</t>
-  </si>
-  <si>
-    <t>352362519</t>
-  </si>
-  <si>
-    <t>behind</t>
-  </si>
-  <si>
-    <t>force to operate behind enemy lines in the [[North African Campaign]]</t>
-  </si>
-  <si>
-    <t>250401991</t>
-  </si>
-  <si>
-    <t>The_Holocaust</t>
-  </si>
-  <si>
-    <t>12323</t>
-  </si>
-  <si>
-    <t>481274320</t>
-  </si>
-  <si>
-    <t>Yad</t>
-  </si>
-  <si>
-    <t>1935|publisher=Yad Vashem}}&lt;/ref&gt;</t>
-  </si>
-  <si>
-    <t>137108568</t>
-  </si>
-  <si>
-    <t>1985, Holmes and Meier Publishers, Inc.</t>
-  </si>
-  <si>
-    <t>188536534</t>
-  </si>
-  <si>
-    <t>over</t>
-  </si>
-  <si>
-    <t>being set up, under whose rulings over 400,000 people were sterilized against</t>
-  </si>
-  <si>
-    <t>392832255</t>
-  </si>
-  <si>
-    <t>escape was impossible for most of them, they</t>
-  </si>
-  <si>
-    <t>170078762</t>
-  </si>
-  <si>
-    <t>Nazi</t>
-  </si>
-  <si>
-    <t>targeted by various deliberate actions by Nazi Germany and</t>
-  </si>
-  <si>
-    <t>287529321</t>
-  </si>
-  <si>
-    <t>party</t>
-  </si>
-  <si>
-    <t>the party's racism. Many leaders of German</t>
-  </si>
-  <si>
-    <t>226617182</t>
-  </si>
-  <si>
-    <t>Toshitsugu_Takamatsu</t>
-  </si>
-  <si>
-    <t>366</t>
-  </si>
-  <si>
-    <t>481179988</t>
-  </si>
-  <si>
-    <t>also</t>
-  </si>
-  <si>
-    <t>genealogy are also made older than they actually are.</t>
-  </si>
-  <si>
-    <t>460127310</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>(Chosui) Takamatsu, also known as Moko no Tora</t>
-  </si>
-  <si>
-    <t>135003903</t>
-  </si>
-  <si>
-    <t>historical</t>
-  </si>
-  <si>
-    <t>have a lineage related to the historical ninja in Japan</t>
-  </si>
-  <si>
-    <t>455245816</t>
-  </si>
-  <si>
-    <t>Prefecture{{citation needed|date=December 2011}}.</t>
-  </si>
-  <si>
-    <t>467046514</t>
-  </si>
-  <si>
-    <t>students. He was the bodyguard</t>
-  </si>
-  <si>
-    <t>139817862</t>
-  </si>
-  <si>
-    <t>Tokyo Times newspaper. He was well known in [[Japan]] as a grandmaster</t>
-  </si>
-  <si>
-    <t>198215859</t>
-  </si>
-  <si>
-    <t>Vladimir_Putin</t>
-  </si>
-  <si>
-    <t>8835</t>
-  </si>
-  <si>
-    <t>481565575</t>
-  </si>
-  <si>
-    <t>They have two daughters, Mariya Putina (born 28 April 1985 in</t>
-  </si>
-  <si>
-    <t>13710123</t>
-  </si>
-  <si>
-    <t>did</t>
-  </si>
-  <si>
-    <t>Boris Yeltsin, Putin did not choose ministers himself</t>
-  </si>
-  <si>
-    <t>376922596</t>
-  </si>
-  <si>
-    <t>Russian company [[Gazprom]] to halt its deliveries of [[natural gas]]</t>
-  </si>
-  <si>
-    <t>264976312</t>
-  </si>
-  <si>
-    <t>included</t>
-  </si>
-  <si>
-    <t>major infrastructure projects]] which he endorsed have included the construction of several major</t>
-  </si>
-  <si>
-    <t>452270016</t>
-  </si>
-  <si>
-    <t>[[Vladimir Gusinsky]], [[Mikhail Khodorkovsky</t>
-  </si>
-  <si>
-    <t>480200996</t>
-  </si>
-  <si>
-    <t>ports of the [[Baltic states]].</t>
-  </si>
-  <si>
-    <t>Wernher_von_Braun</t>
-  </si>
-  <si>
-    <t>2886</t>
-  </si>
-  <si>
-    <t>481374609</t>
-  </si>
-  <si>
-    <t>deceleration intended to commence only a few hundred kilometers above</t>
-  </si>
-  <si>
-    <t>331257357</t>
-  </si>
-  <si>
-    <t>glacial</t>
-  </si>
-  <si>
-    <t>the barren Antarctic terrain like the glacial dry valleys to test the equipment</t>
-  </si>
-  <si>
-    <t>181562429</t>
-  </si>
-  <si>
-    <t>extent</t>
-  </si>
-  <si>
-    <t>Von Braun continued his work to the extent possible, which included</t>
-  </si>
-  <si>
-    <t>312133982</t>
-  </si>
-  <si>
-    <t>picked labor slaves from the [[Buchenwald concentration camp]], who, he admitted 25 years</t>
-  </si>
-  <si>
-    <t>39337246</t>
-  </si>
-  <si>
-    <t>should</t>
-  </si>
-  <si>
-    <t>with unmistakable harshness that I should mind my own business, or find myself</t>
-  </si>
-  <si>
-    <t>60940361</t>
-  </si>
-  <si>
-    <t>=Merk, Otto|title=The Birth of the Missile:The Secrets of Peenemünde</t>
-  </si>
-  <si>
-    <t>278165210</t>
-  </si>
-  <si>
-    <t>carpenter</t>
-  </si>
-  <si>
-    <t>(τέκτων in Greek), usually understood to mean [[carpenter]].</t>
-  </si>
-  <si>
-    <t>78808950</t>
-  </si>
-  <si>
-    <t>sensationalised</t>
-  </si>
-  <si>
-    <t>event at first suppressed, then sensationalised, by the world media</t>
-  </si>
-  <si>
-    <t>46525</t>
-  </si>
-  <si>
-    <t>west</t>
-  </si>
-  <si>
-    <t>(publisher)|West Publishing]]</t>
-  </si>
-  <si>
-    <t>237553561</t>
-  </si>
-  <si>
-    <t>electrolysis</t>
-  </si>
-  <si>
-    <t>The electrolysis of chloride solutions</t>
-  </si>
-  <si>
-    <t>2548818</t>
+    <t xml:space="preserve">448599226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Hues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">462751809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he was one of the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251139604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[circumnavigation|circumnavigated]] the globe with Cavendish between 1586 and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printer to the Queen's Most Excellent Majestie|year=1589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cui solator accessit in arca Londinensi. Quo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generally believed to be an error as no such person was known</t>
+  </si>
+  <si>
+    <t xml:space="preserve">critiqued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page=123|oclc=1981442}}, critiqued by Shirley, ''Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">292186344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturn's_moons_in_fiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">566618655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survivors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find possible survivors transmitting a distress signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">506114944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the Librarium Daemonicum, a repositary of the knowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">138184340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* "Outpost of the Eons" by Dirk Wylie (pseudonym of Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">419171504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourcebook ''GURPS Space: Terradyne'', the Terradyne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">477980732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Image:Dione color south.jpg|right|80px|Dione]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135546415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of human colonization and mining called "M-Base".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127975759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sergei Korolev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">479371650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sergei Korolev.jpg|Image of 1969, 10k stamp.]][</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140290515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gagarin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[http://astrotalkuk.org/2011/07/25/yuri-gagarin-statue-in-london/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">444607919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quality checks. It was successfully launched on 3 November and the dog was placed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14531720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vladimirov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonid Vladimirov related the following description of Korolev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14836512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">world's first space walk. The flight very nearly ended in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yegorov and Feoktistov, was launched</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South_Western_main_line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480564534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[London Waterloo station|Waterloo]] in the centre of London.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">181667862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==References== {{reflist}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">392467433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Railway]] was also formed and built a line from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184072496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basingstoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading to Portsmouth via Basingstoke and Alton but the L&amp;SWR found a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">189287121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The majority of passenger services are currently operated by [[South West Trains]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9375284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use its own track but, after it fell into financial difficulties,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Air Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">572817007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">squadrons, one [[Free French]], one [[Sacred Band</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350603320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lewes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designed by Lieutenant [[Jock Lewes]] and based on the stylised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98628757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 March 2010|publisher=Ministry of Defence|title=Why Join the Royal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">351942186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| 'B' Squadron&lt;ref&gt;Fremont-Barnes, p.4&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael E|title=Encyclopaedia of Elite Forces in the Second World War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">352362519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">behind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">force to operate behind enemy lines in the [[North African Campaign]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250401991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The_Holocaust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481274320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1935|publisher=Yad Vashem}}&lt;/ref&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">137108568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1985, Holmes and Meier Publishers, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188536534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">being set up, under whose rulings over 400,000 people were sterilized against</t>
+  </si>
+  <si>
+    <t xml:space="preserve">392832255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escape was impossible for most of them, they</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170078762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">targeted by various deliberate actions by Nazi Germany and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">287529321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the party's racism. Many leaders of German</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226617182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toshitsugu_Takamatsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481179988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genealogy are also made older than they actually are.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460127310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Chosui) Takamatsu, also known as Moko no Tora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135003903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have a lineage related to the historical ninja in Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455245816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefecture{{citation needed|date=December 2011}}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">467046514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">students. He was the bodyguard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139817862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokyo Times newspaper. He was well known in [[Japan]] as a grandmaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198215859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vladimir_Putin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481565575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They have two daughters, Mariya Putina (born 28 April 1985 in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13710123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">did</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boris Yeltsin, Putin did not choose ministers himself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376922596</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russian company [[Gazprom]] to halt its deliveries of [[natural gas]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264976312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major infrastructure projects]] which he endorsed have included the construction of several major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">452270016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Vladimir Gusinsky]], [[Mikhail Khodorkovsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480200996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ports of the [[Baltic states]].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wernher_von_Braun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">481374609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deceleration intended to commence only a few hundred kilometers above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">331257357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glacial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the barren Antarctic terrain like the glacial dry valleys to test the equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">181562429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Von Braun continued his work to the extent possible, which included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">312133982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picked labor slaves from the [[Buchenwald concentration camp]], who, he admitted 25 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39337246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">should</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with unmistakable harshness that I should mind my own business, or find myself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60940361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=Merk, Otto|title=The Birth of the Missile:The Secrets of Peenemünde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">278165210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carpenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(τέκτων in Greek), usually understood to mean [[carpenter]].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78808950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensationalised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event at first suppressed, then sensationalised, by the world media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">west</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(publisher)|West Publishing]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">237553561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electrolysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The electrolysis of chloride solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2548818</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2322,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="8">
@@ -2582,28 +2593,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:241"/>
+  <dimension ref="A1:AMJ241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A206" activeCellId="0" sqref="A206"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A147" activeCellId="0" sqref="A147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.015306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.0714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="150.811224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="150.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8679,7 +8690,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>